<commit_message>
Added in Vampire class skills doc 5 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/9-Vampire/Documentation/VampireSkills.xlsx
+++ b/GameDesign/Class/9-Vampire/Documentation/VampireSkills.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\9-Vampire\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
+    <sheet name="1-Bite" sheetId="1" r:id="rId1"/>
+    <sheet name="2-BatsSwarm" sheetId="2" r:id="rId2"/>
+    <sheet name="3-ShadowControl" sheetId="3" r:id="rId3"/>
+    <sheet name="4-BloodTransfusion" sheetId="4" r:id="rId4"/>
+    <sheet name="5-VampireMark" sheetId="5" r:id="rId5"/>
     <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -90,6 +90,144 @@
   </si>
   <si>
     <t>[[Number of turns between two casts: -  ]]</t>
+  </si>
+  <si>
+    <t>Bite</t>
+  </si>
+  <si>
+    <t>[[AP: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell ]]</t>
+  </si>
+  <si>
+    <t>Enemies: [[Damage:  40-45 fire ]]</t>
+  </si>
+  <si>
+    <t>Allies:     [[Damage:  50-55 fire ]]</t>
+  </si>
+  <si>
+    <t>Stealth Dark-type health.                                                                More effective on allies player</t>
+  </si>
+  <si>
+    <t>Bats Swarm</t>
+  </si>
+  <si>
+    <t>[[AP: 5 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-5 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: No ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>Teleport the caster at the targeted cell.</t>
+  </si>
+  <si>
+    <t>[[Melee Invulnerable]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Automatically end turn.</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 5 ]]</t>
+  </si>
+  <si>
+    <t>Teleports to the targeted cell and become invulnarable from melee damage.                                                                                             End the turn.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Melee Invulnerable''.</t>
+  </si>
+  <si>
+    <t>Shadow Control</t>
+  </si>
+  <si>
+    <t>[[Range: 2-3 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  35-40 dark ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflicts Dark-type damage. </t>
+  </si>
+  <si>
+    <t>Blood Transfusion</t>
+  </si>
+  <si>
+    <t>Caster: [[-10% caster HP]]</t>
+  </si>
+  <si>
+    <t>Caster: [[-10% caster Max HP]]</t>
+  </si>
+  <si>
+    <t>Target: [[+20% caster Max HP]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-2 ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Void''.</t>
+  </si>
+  <si>
+    <t>Heal the target depending of the caster Max HP.                              The caster life expectancy is reduced.</t>
+  </si>
+  <si>
+    <t>Vampire Mark</t>
+  </si>
+  <si>
+    <t>Effect name: ''Vampire Mark''.</t>
+  </si>
+  <si>
+    <t>Target: [[''Vampire Mark'' effect]] (3 turns)</t>
+  </si>
+  <si>
+    <t>If under ""Blood Moon"" effect:</t>
+  </si>
+  <si>
+    <t>Else:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Target: [[Damage:  20 fire ]] (3 turns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Target: [[Damage:  30 fire ]] (3 turns)</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 3 ]]</t>
+  </si>
+  <si>
+    <t>Poisons that inflicts Fire-type damage.                                                   The poison is stronger if the caster is under ''Blood Moon'' effect.</t>
   </si>
 </sst>
 </file>
@@ -155,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -172,11 +310,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -200,6 +390,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +734,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -546,43 +743,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -594,71 +789,63 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -669,59 +856,13 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="10"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +1112,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -980,138 +1121,130 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1120,42 +1253,17 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1165,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1296,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1197,182 +1305,133 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1382,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1464,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1414,69 +1473,67 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1488,108 +1545,70 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1599,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1641,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1631,69 +1650,67 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1705,14 +1722,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1724,45 +1741,47 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1792,21 +1811,14 @@
     <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
       <c r="C31" s="10" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in Vampire skills doc 3 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/9-Vampire/Documentation/VampireSkills.xlsx
+++ b/GameDesign/Class/9-Vampire/Documentation/VampireSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1-Bite" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="3-ShadowControl" sheetId="3" r:id="rId3"/>
     <sheet name="4-BloodTransfusion" sheetId="4" r:id="rId4"/>
     <sheet name="5-VampireMark" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
+    <sheet name="6-ShadowSpear" sheetId="6" r:id="rId6"/>
+    <sheet name="7-Coffin" sheetId="7" r:id="rId7"/>
+    <sheet name="8-AuraOfTerror" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
     <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -228,6 +228,75 @@
   </si>
   <si>
     <t>Poisons that inflicts Fire-type damage.                                                   The poison is stronger if the caster is under ''Blood Moon'' effect.</t>
+  </si>
+  <si>
+    <t>Shadow Spear</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  30-60 dark ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  20 dark ]] (2 turns)</t>
+  </si>
+  <si>
+    <t>Push 1 cell in the opposite direction of the spell cast point.</t>
+  </si>
+  <si>
+    <t>Inflicts Dark-type damage and Dark-type poison damage.                                                                                           Push the target.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Poison''.</t>
+  </si>
+  <si>
+    <t>Coffin</t>
+  </si>
+  <si>
+    <t>Target: [[Invulnerable]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Invulnerable''.</t>
+  </si>
+  <si>
+    <t>[[AP: 6 ]]</t>
+  </si>
+  <si>
+    <t>Self target:    End turn.</t>
+  </si>
+  <si>
+    <t>Other target: Skip next turn (1 turn)</t>
+  </si>
+  <si>
+    <t>[[Range: 0-2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 1 ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make the target invulnarable and skip his turn.   </t>
+  </si>
+  <si>
+    <t>Aura Of Terror</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 5  ]]</t>
+  </si>
+  <si>
+    <t>[[Aura of Terror]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Aura of Terror''.</t>
+  </si>
+  <si>
+    <t>Entity adjacent of the target: Push the target by 1 cell. (1 turn)</t>
+  </si>
+  <si>
+    <t>All the adjacent entity of the target are pushed away.                               When the entity whit ''Aura of Terror'' move, all the entity adjacent of him get pushed away.                                                                       When an entity move on a cell adjacent of the entity whit ''Aura of Terror'', the entity is pushed away.</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1828,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,7 +1920,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1860,69 +1929,67 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1934,108 +2001,70 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2045,10 +2074,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,7 +2097,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2077,119 +2106,119 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="C16" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2198,61 +2227,35 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2262,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2285,7 +2288,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2294,182 +2297,142 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>